<commit_message>
agregando variable p para guardar datos entre paginas
</commit_message>
<xml_diff>
--- a/WalmartCasosPrueba.xlsx
+++ b/WalmartCasosPrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvvq373\repo\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB320AD2-23CB-4FA4-9DF2-BE31B05CB0C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B75CFF-6BD9-4A95-A19A-8277EDABD816}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,31 +82,13 @@
     <t>Buscar y agregar 1 articulo a la bolsa</t>
   </si>
   <si>
-    <t>producto:case para iphone
-producto: tenis adidas
-numeroProducto: 1
-elegir segundo producto de la lista
-Producto: salsa
-Nombre articulo
-Marca
-precio</t>
-  </si>
-  <si>
     <t xml:space="preserve">LandingPage
 walmartLogo; //css=[class*=header_walmartLogo]
 initialProducts; //id="scrollContainer"
 </t>
   </si>
   <si>
-    <t>CartPage:
-botonCarrito: //css="[data-automation-id='go-to-cart']"
-listaArticulos;//
-mosaicoArticulo;//
-nombreArticulo;//
-precioArticulo;//</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchPage: 
+    <t>SearchPage: 
 searchBar; //css="[class*=searchBarContainer] input"
 searchIcon; //css="button[data-automation-id='search-icon']"
 ResultsPage:
@@ -120,7 +102,26 @@
 precioArticulo; //css="[data-automation-id='list-price'] span"
 addToCart; //css="[data-automation-id='add-button']"
 productAddedValidation; //css="[data-automation-id='add-button']"
-</t>
+botonCarrito: //css="[data-automation-id='add-button']"</t>
+  </si>
+  <si>
+    <t>CartPage:
+verificarProdAgregados; //css="[data-automation-id='added-to-cart']"
+botonCarrito: //css="[data-automation-id='go-to-cart']"
+listaArticulos;//
+mosaicoArticulo;//
+nombreArticulo;//
+precioArticulo;//</t>
+  </si>
+  <si>
+    <t>producto:case para iphone
+producto: tenis adidas
+numeroProducto: 1
+elegir segundo producto de la lista
+Producto: nintendo
+Nombre articulo
+Marca
+precio</t>
   </si>
 </sst>
 </file>
@@ -591,7 +592,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="273.60000000000002">
@@ -603,10 +604,10 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -656,7 +657,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15.05"/>
@@ -711,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="86.4">
+    <row r="7" spans="1:5" ht="100.8">
       <c r="A7" s="5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update a los test scripts
</commit_message>
<xml_diff>
--- a/WalmartCasosPrueba.xlsx
+++ b/WalmartCasosPrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvvq373\repo\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B75CFF-6BD9-4A95-A19A-8277EDABD816}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD05C49-3659-4DC7-8CAE-76D1F7AFB4F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductSearchAdd" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -122,6 +122,16 @@
 Nombre articulo
 Marca
 precio</t>
+  </si>
+  <si>
+    <t>Borrar producto</t>
+  </si>
+  <si>
+    <t>El producto se elimina</t>
+  </si>
+  <si>
+    <t>CartPage:
+deleteButton; //css="[data-automation-id='delete-button']"</t>
   </si>
 </sst>
 </file>
@@ -524,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941B164B-57B5-47A8-B908-90A18B3F7B93}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -656,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82231C9B-F145-4305-AC6B-50E86525E493}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15.05"/>
@@ -727,13 +737,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="30.05">
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="5"/>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">

</xml_diff>